<commit_message>
minor data name fixes
</commit_message>
<xml_diff>
--- a/data/raw_data/data.xlsx
+++ b/data/raw_data/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="satisfied" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="91">
   <si>
     <t>indicator</t>
   </si>
@@ -250,9 +250,6 @@
     <t>youth activities</t>
   </si>
   <si>
-    <t>cemetery maintenace</t>
-  </si>
-  <si>
     <t>problem</t>
   </si>
   <si>
@@ -292,7 +289,7 @@
     <t>poor electricity supply</t>
   </si>
   <si>
-    <t>poorly functioning rubbish collection service </t>
+    <t>poorly functioning rubbish collection service</t>
   </si>
 </sst>
 </file>
@@ -392,13 +389,14 @@
   </sheetPr>
   <dimension ref="A1:AO152"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A54" activeCellId="0" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.5296296296296"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17646,13 +17644,14 @@
   </sheetPr>
   <dimension ref="A1:AO152"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A1 A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.5296296296296"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18029,7 +18028,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2012</v>
@@ -18151,7 +18150,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2015</v>
@@ -34898,7 +34897,7 @@
   <dimension ref="A1:AO23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A1 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34908,7 +34907,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
@@ -35033,7 +35032,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2015</v>
@@ -35137,7 +35136,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2015</v>
@@ -35148,7 +35147,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2015</v>
@@ -35267,7 +35266,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2015</v>
@@ -35284,7 +35283,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>2015</v>
@@ -35346,7 +35345,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>2015</v>
@@ -35414,7 +35413,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>2015</v>
@@ -35428,7 +35427,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>2015</v>
@@ -35448,7 +35447,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2015</v>
@@ -35459,7 +35458,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>2012</v>
@@ -35485,7 +35484,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>2012</v>
@@ -35520,7 +35519,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>2012</v>
@@ -35531,7 +35530,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>2012</v>
@@ -35545,7 +35544,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>2012</v>
@@ -35667,7 +35666,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>2012</v>
@@ -35678,7 +35677,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>2012</v>
@@ -35719,7 +35718,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>2012</v>
@@ -35772,7 +35771,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>2012</v>
@@ -35783,7 +35782,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>2012</v>
@@ -35851,7 +35850,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>2012</v>
@@ -35898,7 +35897,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>2012</v>
@@ -35915,7 +35914,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>2012</v>

</xml_diff>